<commit_message>
Central fed. dist. 10-11 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/cities11-12/1/d11.xlsx
+++ b/migforecasting/cities11-12/1/d11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities11-12\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,9 +22,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="100">
   <si>
     <t>Балашиха</t>
-  </si>
-  <si>
-    <t>Домоде-дово</t>
   </si>
   <si>
     <t>Железнодорожный</t>
@@ -530,6 +527,9 @@
       </rPr>
       <t>12)</t>
     </r>
+  </si>
+  <si>
+    <t>Домодедово</t>
   </si>
 </sst>
 </file>
@@ -556,6 +556,8 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -997,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,61 +1048,61 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
       <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>45</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>46</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>47</v>
-      </c>
-      <c r="V2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1173,37 +1175,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -1222,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6">
         <v>221.8</v>
@@ -1290,7 +1292,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1318,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6">
         <v>33.4</v>
@@ -1386,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6">
         <v>13.4</v>
@@ -1454,7 +1456,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6">
         <v>144.69999999999999</v>
@@ -1522,7 +1524,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6">
         <v>43.7</v>
@@ -1590,7 +1592,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="6">
         <v>13</v>
@@ -1659,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6">
         <v>11.3</v>
@@ -1729,7 +1731,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="6">
         <v>1.7</v>
@@ -1798,7 +1800,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6">
         <v>4762</v>
@@ -1868,7 +1870,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -1892,7 +1894,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="10">
         <v>30.8</v>
@@ -1962,10 +1964,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="10">
         <v>284</v>
@@ -1986,7 +1988,7 @@
         <v>326</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17" s="10">
         <v>698</v>
@@ -2032,7 +2034,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10">
         <v>653</v>
@@ -2102,67 +2104,67 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="W19" s="12"/>
     </row>
@@ -2171,7 +2173,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="10">
         <v>31355</v>
@@ -2240,7 +2242,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="10">
         <v>8954</v>
@@ -2273,7 +2275,7 @@
         <v>9350</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N21" s="10">
         <v>8521</v>
@@ -2309,7 +2311,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="10">
         <v>46.1</v>
@@ -2336,13 +2338,13 @@
         <v>50.8</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L22" s="10">
         <v>31.4</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N22" s="10">
         <v>36</v>
@@ -2378,7 +2380,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="10">
         <v>24</v>
@@ -2402,13 +2404,13 @@
         <v>31.5</v>
       </c>
       <c r="J23" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="L23" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="M23" s="10">
         <v>28.3</v>
@@ -2420,7 +2422,7 @@
         <v>28.6</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q23" s="10">
         <v>24.8</v>
@@ -2435,7 +2437,7 @@
         <v>30.8</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V23" s="10">
         <v>21.1</v>
@@ -2448,7 +2450,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="10">
         <v>43</v>
@@ -2517,7 +2519,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2546,7 +2548,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="10">
         <v>7.1</v>
@@ -2615,7 +2617,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="10">
         <v>6.6</v>
@@ -2684,7 +2686,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -2713,7 +2715,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="10">
         <v>868</v>
@@ -2782,7 +2784,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="10">
         <v>39.1</v>
@@ -2851,7 +2853,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -2880,7 +2882,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="10">
         <v>1421</v>
@@ -2950,7 +2952,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="10">
         <v>64.099999999999994</v>
@@ -3019,7 +3021,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="10">
         <v>6</v>
@@ -3090,7 +3092,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -3120,7 +3122,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="10">
         <v>2.1</v>
@@ -3190,7 +3192,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="10">
         <v>94.7</v>
@@ -3260,7 +3262,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="10">
         <v>20</v>
@@ -3331,7 +3333,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -3361,7 +3363,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="10">
         <v>5.5</v>
@@ -3431,7 +3433,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="10">
         <v>249.4</v>
@@ -3501,13 +3503,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42" s="10">
         <v>1543</v>
@@ -3525,10 +3527,10 @@
         <v>1905</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L42" s="10">
         <v>1964</v>
@@ -3546,10 +3548,10 @@
         <v>1145</v>
       </c>
       <c r="Q42" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R42" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S42" s="10">
         <v>1699</v>
@@ -3571,13 +3573,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43" s="10">
         <v>753</v>
@@ -3595,7 +3597,7 @@
         <v>543</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K43" s="10">
         <v>1416</v>
@@ -3616,10 +3618,10 @@
         <v>419</v>
       </c>
       <c r="Q43" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R43" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S43" s="10">
         <v>554</v>
@@ -3641,67 +3643,67 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V44" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W44" s="12"/>
     </row>
@@ -3711,7 +3713,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="10">
         <v>35430</v>
@@ -3782,7 +3784,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="10">
         <v>4774</v>
@@ -3853,7 +3855,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="10">
         <v>37.5</v>
@@ -3923,7 +3925,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="10">
         <v>9.9</v>
@@ -3993,67 +3995,67 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V49" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W49" s="12"/>
     </row>
@@ -4063,7 +4065,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="10">
         <v>5912</v>
@@ -4133,7 +4135,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -4163,7 +4165,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -4194,52 +4196,52 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G53" s="10">
         <v>5</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R53" s="13">
         <v>1</v>
@@ -4248,7 +4250,7 @@
         <v>1</v>
       </c>
       <c r="T53" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U53" s="13">
         <v>2</v>
@@ -4265,7 +4267,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="10">
         <v>39</v>
@@ -4336,7 +4338,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="10">
         <v>6</v>
@@ -4407,7 +4409,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -4437,67 +4439,67 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G57" s="10">
         <v>192.5</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R57" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S57" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T57" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U57" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V57" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W57" s="12"/>
     </row>
@@ -4507,7 +4509,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="10">
         <v>12852.1</v>
@@ -4577,7 +4579,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="10">
         <v>4071.3</v>
@@ -4647,37 +4649,37 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L60" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
@@ -4697,7 +4699,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="10">
         <v>1058.5999999999999</v>
@@ -4748,7 +4750,7 @@
         <v>2480.4</v>
       </c>
       <c r="S61" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T61" s="13">
         <v>2487.9</v>
@@ -4767,7 +4769,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -4797,7 +4799,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="10">
         <v>650.5</v>
@@ -4867,7 +4869,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="10">
         <v>9682</v>
@@ -4946,13 +4948,13 @@
         <v>125</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I65" s="10">
         <v>440</v>
@@ -4961,40 +4963,40 @@
         <v>220</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L65" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O65" s="13">
         <v>420</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T65" s="13">
         <v>355</v>
       </c>
       <c r="U65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V65" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W65" s="12"/>
     </row>
@@ -5064,7 +5066,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -5094,7 +5096,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="13">
         <v>18246.599999999999</v>
@@ -5164,7 +5166,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C71" s="13">
         <v>103.5</v>
@@ -5234,7 +5236,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" s="13">
         <v>543.4</v>
@@ -5304,7 +5306,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" s="13">
         <v>104.7</v>
@@ -5374,7 +5376,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W74" s="12"/>
     </row>
@@ -5384,7 +5386,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C75" s="13">
         <v>2094.4</v>
@@ -5454,7 +5456,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76" s="13">
         <v>11.7</v>
@@ -5511,7 +5513,7 @@
         <v>10.5</v>
       </c>
       <c r="U76" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V76" s="10">
         <v>4.3</v>
@@ -5524,7 +5526,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -5554,7 +5556,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78" s="13">
         <v>6.3</v>
@@ -5575,10 +5577,10 @@
         <v>10.9</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K78" s="13">
         <v>0.2</v>
@@ -5587,7 +5589,7 @@
         <v>13.1</v>
       </c>
       <c r="M78" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N78" s="10">
         <v>0.4</v>
@@ -5611,7 +5613,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="U78" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V78" s="10">
         <v>2.0499999999999998</v>
@@ -5624,7 +5626,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="13">
         <v>4.8</v>
@@ -5633,7 +5635,7 @@
         <v>0.3</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F79" s="13">
         <v>0.7</v>
@@ -5681,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="U79" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V79" s="10">
         <v>2.0299999999999998</v>
@@ -5691,7 +5693,7 @@
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W80" s="12"/>
     </row>

</xml_diff>